<commit_message>
update db_dict to include tbl_pesquisador_ave, fix logic model and sql script
Signed-off-by: Nelson Buainain <nnbuainain@gmail.com>
</commit_message>
<xml_diff>
--- a/DB_Dictionary/db_dictionary.xlsx
+++ b/DB_Dictionary/db_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnbuainain/Dropbox/Data_Science/Projects/database_inpa_crg/DB_Dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE35BCC-24C5-C944-A4FF-4B191D8430D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC66EAC-9551-2B41-9089-97896E521069}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" activeTab="2" xr2:uid="{898E14BC-01F6-D247-AB48-0AC14AE1D90A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="204">
   <si>
     <t>Tabela</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Descricao</t>
   </si>
   <si>
-    <t>Escreve</t>
-  </si>
-  <si>
     <t>Nome da Coluna</t>
   </si>
   <si>
@@ -56,18 +53,9 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>tbl_livro</t>
-  </si>
-  <si>
     <t>FK</t>
   </si>
   <si>
-    <t>tbl_autor</t>
-  </si>
-  <si>
-    <t>Autor que escreve livro</t>
-  </si>
-  <si>
     <t>tbl_Amostra</t>
   </si>
   <si>
@@ -86,9 +74,6 @@
     <t>tbl_Herpeto</t>
   </si>
   <si>
-    <t>tbl_Aves</t>
-  </si>
-  <si>
     <t>tbl_Peixe</t>
   </si>
   <si>
@@ -630,6 +615,30 @@
   </si>
   <si>
     <t>Instituição atual a qual pertence o pesquisador</t>
+  </si>
+  <si>
+    <t>tbl_Pesquisador_Ave</t>
+  </si>
+  <si>
+    <t>Tabela para cadastro de relação um pra um entre Pesquisadores e Coletores de especimes Voucher (animal fisico e não amostra genética)</t>
+  </si>
+  <si>
+    <t>Relação um pra um entre Pesquisadores que coletam espécimes de aves do tipo Voucher (animal fisico e não amostra genética)</t>
+  </si>
+  <si>
+    <t>id_pesq_ave</t>
+  </si>
+  <si>
+    <t>Número único que identifica uma relação única entre pesquisadores que são coletores de espécimes de aves do tipo Voucher (animal físico e não amostra genética)</t>
+  </si>
+  <si>
+    <t>Número sequencial único que identifica um pesquisador na tbl_Pesquisador. Aqui é usado como chave estrangeira como ligação com a tbl_Pesquisador</t>
+  </si>
+  <si>
+    <t>Data de coleta da amostra genética</t>
+  </si>
+  <si>
+    <t>VARCHAR (60)</t>
   </si>
 </sst>
 </file>
@@ -702,9 +711,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -718,9 +724,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -728,21 +731,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,417 +1066,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3F929E-88DE-964D-B186-6EADBF25D50E}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="123.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D8" s="16"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D11" s="16"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="D15" s="5"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="D17" s="4"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="D21" s="7"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="D24" s="7"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" ht="17">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" ht="17">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" ht="34">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="D28" s="7"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" ht="34">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="17">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="D33" s="7"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>47</v>
+        <v>19</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="B35" t="s">
-        <v>45</v>
+        <v>196</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="D36" s="7"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="D39" s="8"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="12"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D37:D38"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D37:D38"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1475,256 +1511,270 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F442F6-671F-1E4C-8568-6FA98FA3BB5B}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="109.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1734,908 +1784,962 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFED671A-AD9D-A542-8629-2639FB35C597}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5" customWidth="1"/>
+    <col min="7" max="7" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="17"/>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="17"/>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="17"/>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="17"/>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="17"/>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="13" t="s">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="17"/>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
         <v>73</v>
       </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="14"/>
-      <c r="B3" t="s">
+      <c r="E12" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="17"/>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="17"/>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
         <v>73</v>
       </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="14"/>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
         <v>73</v>
       </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="14"/>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="14"/>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="17"/>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="15"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="14"/>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="17"/>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="10"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
         <v>96</v>
       </c>
-      <c r="G9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="14"/>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="17"/>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="15"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="14"/>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="17"/>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="17"/>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="17"/>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="17"/>
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="14"/>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="15"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="14"/>
-      <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="14"/>
-      <c r="B18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="15"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="14"/>
-      <c r="B21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="14"/>
-      <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
         <v>110</v>
       </c>
-      <c r="G24" t="s">
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="17"/>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="17"/>
+      <c r="B31" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="14"/>
-      <c r="B25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="14"/>
-      <c r="B26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="14"/>
-      <c r="B27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="14"/>
-      <c r="B30" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" t="s">
-        <v>123</v>
-      </c>
-      <c r="G30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="14"/>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
         <v>117</v>
-      </c>
-      <c r="C31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G33" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G34" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" t="s">
         <v>129</v>
-      </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" t="s">
         <v>130</v>
-      </c>
-      <c r="C37" t="s">
-        <v>123</v>
-      </c>
-      <c r="G37" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" t="s">
         <v>131</v>
-      </c>
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" t="s">
         <v>132</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G41" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="B42" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G42" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="B43" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G43" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G44" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G45" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E47" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G47" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G48" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G50" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="B51" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G51" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="B52" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G52" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="B53" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>203</v>
       </c>
       <c r="G53" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="B54" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G54" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="B55" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G55" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="B56" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G56" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="B57" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G57" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="B58" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G58" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="B59" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>164</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>175</v>
+        <v>159</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="B60" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" t="s">
         <v>159</v>
       </c>
-      <c r="C60" t="s">
-        <v>164</v>
-      </c>
       <c r="G60" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="B61" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G61" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="B62" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G62" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G64" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="B65" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C65" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
       </c>
       <c r="G65" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="B66" t="s">
-        <v>179</v>
+        <v>124</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>118</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
       </c>
       <c r="G66" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="B67" t="s">
-        <v>180</v>
-      </c>
-      <c r="C67" t="s">
-        <v>163</v>
-      </c>
-      <c r="G67" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
       <c r="B68" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C68" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="G68" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="C69" t="s">
         <v>73</v>
       </c>
-      <c r="E69" t="s">
-        <v>10</v>
-      </c>
       <c r="G69" t="s">
-        <v>134</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="B70" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" t="s">
+        <v>158</v>
+      </c>
+      <c r="G70" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>23</v>
-      </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
-      </c>
-      <c r="E71" s="16" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="G71" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="B72" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>73</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="B73" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" t="s">
+        <v>68</v>
+      </c>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" t="s">
         <v>129</v>
       </c>
-      <c r="C73" t="s">
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" t="s">
         <v>73</v>
       </c>
-      <c r="E73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="B74" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" t="s">
-        <v>78</v>
-      </c>
-      <c r="E74" t="s">
-        <v>10</v>
+      <c r="E75" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G75" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>45</v>
-      </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C76" t="s">
-        <v>78</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="G76" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="B77" t="s">
-        <v>186</v>
+        <v>124</v>
       </c>
       <c r="C77" t="s">
-        <v>123</v>
+        <v>68</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
       </c>
       <c r="G77" t="s">
-        <v>197</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C78" t="s">
-        <v>123</v>
+        <v>73</v>
+      </c>
+      <c r="E78" t="s">
+        <v>8</v>
       </c>
       <c r="G78" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="B79" t="s">
-        <v>188</v>
-      </c>
-      <c r="C79" t="s">
-        <v>110</v>
-      </c>
-      <c r="G79" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>40</v>
+      </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
-      </c>
-      <c r="G80" s="17" t="s">
-        <v>200</v>
+        <v>73</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G80" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" t="s">
+        <v>181</v>
+      </c>
+      <c r="C81" t="s">
+        <v>118</v>
+      </c>
+      <c r="G81" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" t="s">
+        <v>118</v>
+      </c>
+      <c r="G82" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" t="s">
+        <v>105</v>
+      </c>
+      <c r="G83" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" t="s">
+        <v>105</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename table pesquisador_ave as coleta_voucher, update model, sql, code and database accordingly
Signed-off-by: Nelson Buainain <nnbuainain@gmail.com>
</commit_message>
<xml_diff>
--- a/DB_Dictionary/db_dictionary.xlsx
+++ b/DB_Dictionary/db_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnbuainain/Dropbox/Data_Science/Projects/database_inpa_crg/DB_Dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC66EAC-9551-2B41-9089-97896E521069}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1545E7-9EE0-D34E-B7F9-61560F0D0BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" activeTab="2" xr2:uid="{898E14BC-01F6-D247-AB48-0AC14AE1D90A}"/>
+    <workbookView xWindow="27640" yWindow="460" windowWidth="25600" windowHeight="14200" activeTab="2" xr2:uid="{898E14BC-01F6-D247-AB48-0AC14AE1D90A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelas" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="217">
   <si>
     <t>Tabela</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Tabela para cadastro do País de origem da amostra</t>
   </si>
   <si>
-    <t>tbl_amostra</t>
-  </si>
-  <si>
     <t>Tabela para cadastro de atributos exclusivos da coleção de Herpetologia</t>
   </si>
   <si>
@@ -158,15 +155,9 @@
     <t>Tabela para cadastro de atributos exclusivos da coleção de Aves</t>
   </si>
   <si>
-    <t>Tabela para cadastro de relações normais entre Coletas de amostras genéticas e Pesquisadores permitindo multiplos valores. Registra quem foi o (s) coletor (es) de cada amostra genética</t>
-  </si>
-  <si>
     <t>Tabela para cadastro de relações normais entre Solicitações de empréstimo e Pesquisadores permitindo multiplos valores. Registra pedidos de solicitação de empréstimo de amostras genéticas</t>
   </si>
   <si>
-    <t xml:space="preserve">Tabela para cadastro de pesquisadores que podem estar associados à amostras genéticas tanto como coletores, quanto como solicitantes de empréstimo, ou ainda como coletor de voucher (espécimes fisicos taxidermixados) no caso de Aves onde essas duas coisas podem não necessariamente coincidir como é o caso dos outros grupos </t>
-  </si>
-  <si>
     <t>Tabela 1 - PL</t>
   </si>
   <si>
@@ -191,9 +182,6 @@
     <t>Estado ao qual uma localidade pertence</t>
   </si>
   <si>
-    <t>Pais ao qual pertence um estado</t>
-  </si>
-  <si>
     <t>Informações adicionais sobre a proveniencia de localidades da coleção de Peixes</t>
   </si>
   <si>
@@ -203,9 +191,6 @@
     <t>Informações adicionais e exclusivas sobre amostras da coleção de Peixes</t>
   </si>
   <si>
-    <t>Informações adicionais e exclusivas  sobre amostras da coleção de Herpetologia</t>
-  </si>
-  <si>
     <t>Relação entre um pedido (por parte de um ou mais pesquisadores) de empréstimo e uma amostra genética</t>
   </si>
   <si>
@@ -458,12 +443,6 @@
     <t>FK_num_amostra</t>
   </si>
   <si>
-    <t>nome_municipio</t>
-  </si>
-  <si>
-    <t>Nome do Municipio mais próximo da localidade em que a amostra da coleção de herpetologia foi coletada</t>
-  </si>
-  <si>
     <t>sexo</t>
   </si>
   <si>
@@ -497,9 +476,6 @@
     <t>subespecie</t>
   </si>
   <si>
-    <t>fk_nome_preparador</t>
-  </si>
-  <si>
     <t>CHAR (1)</t>
   </si>
   <si>
@@ -530,9 +506,6 @@
     <t>Nível taxonomico exclusivo da coleção de aves. Em teoria deveria pertencer a uma única espécie e estar condicionalmente ligada a essa tabela, mas foi mantida aqui para simplificar o banco de dados, e porque essa informação não é coletada de forma sistêmica pelos coletores. Aparece mais como uma observação ou informação esporádica</t>
   </si>
   <si>
-    <t>Número único sequencial que identifica um Pesquisador na tbl_Pesquisador, responsável por coletar o voucher (espécime físico) a qual pertence uma amostra genética. Nas demais coleções, o pesquisador que coleta a amostra genética é sempre o mesmo do espécime físico, porém em aves isso pode variar pois existem amostras que só tem sangue coletado, sem o espécime físico, e existem casos onde um pesquisador coleta o espécime físico, e outro faz o processo de taxidermia e portanto é o responsável por extrair a amostra genética (musculo) do espécime</t>
-  </si>
-  <si>
     <t>Se a amostra é do tipo coração, não é mutualmente exclusiva em relação às demais categorias booleanas</t>
   </si>
   <si>
@@ -584,9 +557,6 @@
     <t>instituicao</t>
   </si>
   <si>
-    <t>Número sequencial único que identifica uma relação entre amostra e uma solicitação de emprestimo</t>
-  </si>
-  <si>
     <t>Número da guia de empréstimo, documentação oficial do INPA com número sequencial único por empréstimo. Um empréstimo é um conjunto ou lote de amostras solicitadas por um pesquisador para realizar seu estudo científico.</t>
   </si>
   <si>
@@ -599,12 +569,6 @@
     <t>Número sequencial único que identifica um pesquisador na tbl_Pesquisador</t>
   </si>
   <si>
-    <t>Número sequencial único que identifica uma relação de solicitação de empréstimo entre um amostra e um pesquisador</t>
-  </si>
-  <si>
-    <t>Número sequencial único que identifica uma relação de coleta/depósito na coleção entre entre uma amostra e um pesquisador</t>
-  </si>
-  <si>
     <t>Nome do Pesquisador</t>
   </si>
   <si>
@@ -617,21 +581,12 @@
     <t>Instituição atual a qual pertence o pesquisador</t>
   </si>
   <si>
-    <t>tbl_Pesquisador_Ave</t>
-  </si>
-  <si>
-    <t>Tabela para cadastro de relação um pra um entre Pesquisadores e Coletores de especimes Voucher (animal fisico e não amostra genética)</t>
-  </si>
-  <si>
     <t>Relação um pra um entre Pesquisadores que coletam espécimes de aves do tipo Voucher (animal fisico e não amostra genética)</t>
   </si>
   <si>
     <t>id_pesq_ave</t>
   </si>
   <si>
-    <t>Número único que identifica uma relação única entre pesquisadores que são coletores de espécimes de aves do tipo Voucher (animal físico e não amostra genética)</t>
-  </si>
-  <si>
     <t>Número sequencial único que identifica um pesquisador na tbl_Pesquisador. Aqui é usado como chave estrangeira como ligação com a tbl_Pesquisador</t>
   </si>
   <si>
@@ -639,6 +594,90 @@
   </si>
   <si>
     <t>VARCHAR (60)</t>
+  </si>
+  <si>
+    <t>tbl_coletor_voucher</t>
+  </si>
+  <si>
+    <t>Tabela para cadastro de atributos exclusivos da coleção de Peixes</t>
+  </si>
+  <si>
+    <t>Tabela para cadastro de relação um pra um entre Pesquisadores e Coletores de especimes Voucher (animal fisico e não amostra genética). Essa relação é exclusiva para aves pois nos demais grupos o coletor da amostra genética é o mesmo do coletor do voucher</t>
+  </si>
+  <si>
+    <t>Tabela para cadastro de relações normais entre Coletas de amostras genéticas e Pesquisadores permitindo multiplos valores. Registra quem foi o (s) coletor (es) de cada amostra genética. Para as coleções de peixes e herpetologia, o coletor da amostra genétia é o mesmo coletor do voucher</t>
+  </si>
+  <si>
+    <t>Tabela para cadastro de pesquisadores que podem estar associados à amostras genéticas tanto como coletores, quanto como solicitantes de empréstimo, ou ainda como coletor de voucher (espécimes fisicos)</t>
+  </si>
+  <si>
+    <t>tbl_coleta_voucher</t>
+  </si>
+  <si>
+    <t>Pais ao qual um estado  pertence</t>
+  </si>
+  <si>
+    <t>municipio</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>VARCHAR (300)</t>
+  </si>
+  <si>
+    <t>identificacao_especie_obs</t>
+  </si>
+  <si>
+    <t>colecao</t>
+  </si>
+  <si>
+    <t>Município do qual vem a amostra</t>
+  </si>
+  <si>
+    <t>Quaisquer observações adicionais sobre a amostra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observações relavantes à identificação da espécie. Pode indicar o nivel de certeza (cf, sp), um grupo superior (gr.), um taxon não descrito (sp1, sp2), etc... </t>
+  </si>
+  <si>
+    <t>Colecao a qual pertence a amostra, se aves, peixes ou herpeto</t>
+  </si>
+  <si>
+    <t>coordenadas_obs</t>
+  </si>
+  <si>
+    <t>Observações sobre as coordenadas. Geralmente indica se coordenada é aproximada mas pode indicar valor incorreto ou qualquer outra observacao relevante</t>
+  </si>
+  <si>
+    <t>Número sequencial único que identifica uma relação entre uma amostra e uma solicitação de emprestimo</t>
+  </si>
+  <si>
+    <t>Número sequencial único que identifica uma relação única entre um pesquisador que é coletor único ou conjunto de um espécime de ave do tipo Voucher (animal físico e não amostra genética)</t>
+  </si>
+  <si>
+    <t>Número sequencial único que identifica uma relação única de solicitação de empréstimo entre uma amostra e um pesquisador</t>
+  </si>
+  <si>
+    <t>Número sequencial único que identifica uma relação única de coleta (depósito) na coleção entre entre uma amostra e um pesquisador</t>
+  </si>
+  <si>
+    <t>sexo_obs</t>
+  </si>
+  <si>
+    <t>Observações relevantes a identificação do sexo da amostra. Pode indicar a incerteza, notações erradas ou fora do padrão, ou simplesmente o dado original antes do tratamento</t>
+  </si>
+  <si>
+    <t>data_preparacao_obs</t>
+  </si>
+  <si>
+    <t>Observações relevantes a data de preparação do especime, geralmente indica se a data foi aproximada quando a data original não continha dia, mes e ano, ou se estava incorreta</t>
+  </si>
+  <si>
+    <t>Observações relevantes a data de coleta da amostra, geralmente indica se a data foi aproximada quando a data original não continha dia, mes e ano, ou se estava incorreta</t>
+  </si>
+  <si>
+    <t>data_coleta_obs</t>
   </si>
 </sst>
 </file>
@@ -709,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -737,6 +776,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1066,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3F929E-88DE-964D-B186-6EADBF25D50E}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:D38"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1104,7 +1146,7 @@
       <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1115,7 +1157,7 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
@@ -1124,7 +1166,7 @@
       <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
@@ -1133,7 +1175,7 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
@@ -1142,7 +1184,7 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
@@ -1151,7 +1193,7 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
@@ -1160,7 +1202,7 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -1172,7 +1214,7 @@
       <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1183,7 +1225,7 @@
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
@@ -1195,7 +1237,7 @@
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1206,7 +1248,7 @@
       <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" s="4"/>
@@ -1238,7 +1280,7 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1249,7 +1291,7 @@
       <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
@@ -1258,7 +1300,7 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4">
       <c r="D21" s="5"/>
@@ -1273,7 +1315,7 @@
       <c r="C22" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="14" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1284,7 +1326,7 @@
       <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4">
       <c r="D24" s="5"/>
@@ -1317,7 +1359,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1333,177 +1375,160 @@
       <c r="C29" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>38</v>
+      <c r="D29" s="14" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="13"/>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4">
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" ht="17">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>38</v>
+      <c r="D32" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="D33" s="5"/>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="14"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
         <v>9</v>
       </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="13" t="s">
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="B35" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="13"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>196</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="B38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="13"/>
-    </row>
     <row r="39" spans="1:4">
-      <c r="D39" s="5"/>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" t="s">
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="14"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="B41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+      <c r="D44" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="C45" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="B44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="13"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="15"/>
+      <c r="D45" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D44:D45"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D35:D36"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1511,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F442F6-671F-1E4C-8568-6FA98FA3BB5B}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1530,10 +1555,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>2</v>
@@ -1550,7 +1575,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1564,7 +1589,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1578,7 +1603,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1592,7 +1617,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1606,7 +1631,7 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1620,7 +1645,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1634,7 +1659,7 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1648,7 +1673,7 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1656,13 +1681,13 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1670,27 +1695,27 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1698,27 +1723,27 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1729,24 +1754,24 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1757,24 +1782,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1784,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFED671A-AD9D-A542-8629-2639FB35C597}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1812,7 +1823,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>5</v>
@@ -1825,751 +1836,755 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="18"/>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="18"/>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="18"/>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="18"/>
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="18"/>
+      <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="18"/>
+      <c r="B8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="18"/>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
         <v>69</v>
       </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="17"/>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="18"/>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
         <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="17"/>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="17"/>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="17"/>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="17"/>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="17"/>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="13"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="18"/>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="18"/>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="18"/>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="18"/>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="10"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="18"/>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="18"/>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="10"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="18"/>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="17"/>
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="18"/>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="18"/>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="18"/>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="18"/>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="18"/>
+      <c r="B33" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="17"/>
-      <c r="B14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" t="s">
         <v>8</v>
       </c>
-      <c r="G14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="10"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="17"/>
-      <c r="B17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="17"/>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="G33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="18"/>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="18"/>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="17"/>
-      <c r="B21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="G37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="B40" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="17"/>
-      <c r="B24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="17"/>
-      <c r="B25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="17"/>
-      <c r="B26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="17"/>
-      <c r="B27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="G40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
         <v>119</v>
       </c>
-      <c r="G29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="17"/>
-      <c r="B30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="17"/>
-      <c r="B31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>120</v>
-      </c>
-      <c r="G33" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="B34" t="s">
-        <v>121</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="G42" t="s">
         <v>124</v>
-      </c>
-      <c r="C36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" t="s">
-        <v>128</v>
-      </c>
-      <c r="G36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="B37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="B38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="B39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="B42" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" t="s">
-        <v>80</v>
-      </c>
-      <c r="G42" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="B43" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="G43" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="G44" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="E45" t="s">
+        <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="G47" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
-        <v>143</v>
+        <v>129</v>
+      </c>
+      <c r="C48" t="s">
+        <v>75</v>
       </c>
       <c r="G48" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>16</v>
-      </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="G50" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="B51" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
       <c r="G51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="B52" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
-      </c>
-      <c r="G52" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C53" t="s">
-        <v>203</v>
+        <v>63</v>
+      </c>
+      <c r="E53" t="s">
+        <v>123</v>
       </c>
       <c r="G53" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="B54" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="G54" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="B55" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="G55" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="B56" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>75</v>
       </c>
       <c r="G56" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="B57" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="G57" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="B58" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="G58" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="B59" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
-        <v>159</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>170</v>
+        <v>113</v>
+      </c>
+      <c r="G59" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="B60" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G60" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="B61" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="C61" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="G61" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="B62" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
-      </c>
-      <c r="E62" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="G62" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" t="s">
+        <v>151</v>
+      </c>
+      <c r="G63" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>196</v>
-      </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E64" t="s">
-        <v>69</v>
-      </c>
-      <c r="G64" t="s">
-        <v>200</v>
+        <v>151</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="B65" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
-        <v>73</v>
-      </c>
-      <c r="E65" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="G65" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="B66" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
-      </c>
-      <c r="E66" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="G66" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B68" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C68" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E68" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G68" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
       </c>
       <c r="G69" t="s">
         <v>186</v>
@@ -2577,180 +2592,233 @@
     </row>
     <row r="70" spans="1:7">
       <c r="B70" t="s">
-        <v>174</v>
+        <v>119</v>
       </c>
       <c r="C70" t="s">
-        <v>158</v>
+        <v>113</v>
+      </c>
+      <c r="E70" t="s">
+        <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="B71" t="s">
-        <v>175</v>
-      </c>
-      <c r="C71" t="s">
-        <v>158</v>
-      </c>
-      <c r="G71" t="s">
-        <v>188</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>17</v>
+      </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E72" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="G72" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="B73" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
         <v>68</v>
       </c>
-      <c r="E73" t="s">
-        <v>8</v>
-      </c>
       <c r="G73" t="s">
-        <v>129</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="B74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" t="s">
+        <v>150</v>
+      </c>
+      <c r="G74" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" t="s">
-        <v>18</v>
-      </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="G75" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="B76" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C76" t="s">
-        <v>158</v>
+        <v>68</v>
+      </c>
+      <c r="E76" t="s">
+        <v>8</v>
       </c>
       <c r="G76" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="B77" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C77" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
       </c>
       <c r="G77" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="B78" t="s">
-        <v>178</v>
-      </c>
-      <c r="C78" t="s">
-        <v>73</v>
-      </c>
-      <c r="E78" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" t="s">
+        <v>68</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G79" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="B80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" t="s">
+        <v>150</v>
+      </c>
+      <c r="G80" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="B81" t="s">
+        <v>216</v>
+      </c>
+      <c r="C81" t="s">
+        <v>75</v>
+      </c>
+      <c r="G81" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="B82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+      <c r="E82" t="s">
         <v>8</v>
       </c>
-      <c r="G78" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
-        <v>40</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="G82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="B83" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B85" t="s">
+        <v>171</v>
+      </c>
+      <c r="C85" t="s">
+        <v>68</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G85" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="B86" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" t="s">
+        <v>113</v>
+      </c>
+      <c r="G86" t="s">
         <v>180</v>
       </c>
-      <c r="C80" t="s">
-        <v>73</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G80" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7">
-      <c r="B81" t="s">
+    </row>
+    <row r="87" spans="1:7">
+      <c r="B87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" t="s">
         <v>181</v>
       </c>
-      <c r="C81" t="s">
-        <v>118</v>
-      </c>
-      <c r="G81" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7">
-      <c r="B82" t="s">
+    </row>
+    <row r="88" spans="1:7">
+      <c r="B88" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" t="s">
+        <v>100</v>
+      </c>
+      <c r="G88" t="s">
         <v>182</v>
       </c>
-      <c r="C82" t="s">
-        <v>118</v>
-      </c>
-      <c r="G82" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7">
-      <c r="B83" t="s">
+    </row>
+    <row r="89" spans="1:7">
+      <c r="B89" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" t="s">
+        <v>100</v>
+      </c>
+      <c r="G89" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="C83" t="s">
-        <v>105</v>
-      </c>
-      <c r="G83" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7">
-      <c r="B84" t="s">
-        <v>184</v>
-      </c>
-      <c r="C84" t="s">
-        <v>105</v>
-      </c>
-      <c r="G84" s="12" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A28:A33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
add columns that were missing to the table peixe, update model and sql accordingly
Signed-off-by: Nelson Buainain <nnbuainain@gmail.com>
</commit_message>
<xml_diff>
--- a/DB_Dictionary/db_dictionary.xlsx
+++ b/DB_Dictionary/db_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnbuainain/Dropbox/Data_Science/Projects/database_inpa_crg/DB_Dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1545E7-9EE0-D34E-B7F9-61560F0D0BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEDE370-77DF-5B48-8475-61420DD8C108}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27640" yWindow="460" windowWidth="25600" windowHeight="14200" activeTab="2" xr2:uid="{898E14BC-01F6-D247-AB48-0AC14AE1D90A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="224">
   <si>
     <t>Tabela</t>
   </si>
@@ -678,6 +678,27 @@
   </si>
   <si>
     <t>data_coleta_obs</t>
+  </si>
+  <si>
+    <t>responsavel_projeto</t>
+  </si>
+  <si>
+    <t>Pesquisador responsável pelo projeto em que a amostra foi coletada</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Status da amostra na coleção. Geralmente indica se a amostra acabou/ se esgotou</t>
+  </si>
+  <si>
+    <t>comprimento_padrão</t>
+  </si>
+  <si>
+    <t>Comprimento do espécime voucher em centimetros</t>
+  </si>
+  <si>
+    <t>DECIMAL (5,2)</t>
   </si>
 </sst>
 </file>
@@ -1795,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFED671A-AD9D-A542-8629-2639FB35C597}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2326,487 +2347,520 @@
     </row>
     <row r="45" spans="1:7">
       <c r="B45" t="s">
-        <v>122</v>
+        <v>217</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
-      </c>
-      <c r="E45" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>127</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="B46" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>27</v>
-      </c>
       <c r="B47" t="s">
-        <v>128</v>
+        <v>221</v>
       </c>
       <c r="C47" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="G47" t="s">
-        <v>132</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="B48" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="B49" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>68</v>
+      </c>
+      <c r="E50" t="s">
+        <v>64</v>
       </c>
       <c r="G50" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G51" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>16</v>
-      </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
-      </c>
-      <c r="E53" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="G53" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="B54" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>68</v>
       </c>
       <c r="G54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="B55" t="s">
-        <v>211</v>
-      </c>
-      <c r="C55" t="s">
-        <v>75</v>
-      </c>
-      <c r="G55" t="s">
-        <v>212</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C56" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="E56" t="s">
+        <v>123</v>
       </c>
       <c r="G56" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="B57" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="G57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="B58" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="G58" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="B59" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="G59" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="B60" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="G60" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="B61" t="s">
-        <v>213</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="G61" t="s">
-        <v>214</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="B62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="G62" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="B63" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G63" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="B64" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="C64" t="s">
-        <v>151</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>161</v>
+        <v>75</v>
+      </c>
+      <c r="G64" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="B65" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
         <v>151</v>
       </c>
       <c r="G65" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="B66" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C66" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="G66" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="B67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" t="s">
+        <v>151</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" t="s">
-        <v>194</v>
-      </c>
       <c r="B68" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="C68" t="s">
-        <v>68</v>
-      </c>
-      <c r="E68" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="G68" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" t="s">
+        <v>113</v>
+      </c>
+      <c r="G69" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>194</v>
+      </c>
+      <c r="B71" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" t="s">
+        <v>68</v>
+      </c>
+      <c r="E71" t="s">
+        <v>64</v>
+      </c>
+      <c r="G71" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="B72" t="s">
         <v>170</v>
-      </c>
-      <c r="C69" t="s">
-        <v>68</v>
-      </c>
-      <c r="E69" t="s">
-        <v>8</v>
-      </c>
-      <c r="G69" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="B70" t="s">
-        <v>119</v>
-      </c>
-      <c r="C70" t="s">
-        <v>113</v>
-      </c>
-      <c r="E70" t="s">
-        <v>8</v>
-      </c>
-      <c r="G70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
-        <v>17</v>
-      </c>
-      <c r="B72" t="s">
-        <v>163</v>
       </c>
       <c r="C72" t="s">
         <v>68</v>
       </c>
       <c r="E72" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="G72" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="B73" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="C73" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" t="s">
         <v>68</v>
       </c>
-      <c r="G73" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="B74" t="s">
-        <v>165</v>
-      </c>
-      <c r="C74" t="s">
-        <v>150</v>
-      </c>
-      <c r="G74" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="B75" t="s">
-        <v>166</v>
-      </c>
-      <c r="C75" t="s">
-        <v>150</v>
+      <c r="E75" t="s">
+        <v>64</v>
       </c>
       <c r="G75" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="B76" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C76" t="s">
         <v>68</v>
       </c>
-      <c r="E76" t="s">
-        <v>8</v>
-      </c>
       <c r="G76" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="B77" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="C77" t="s">
-        <v>63</v>
-      </c>
-      <c r="E77" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="G77" t="s">
-        <v>124</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="B78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" t="s">
+        <v>150</v>
+      </c>
+      <c r="G78" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" t="s">
-        <v>18</v>
-      </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C79" t="s">
         <v>68</v>
       </c>
-      <c r="E79" s="11" t="s">
-        <v>64</v>
+      <c r="E79" t="s">
+        <v>8</v>
       </c>
       <c r="G79" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="B80" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="C80" t="s">
-        <v>150</v>
+        <v>63</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
       </c>
       <c r="G80" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="B81" t="s">
-        <v>216</v>
-      </c>
-      <c r="C81" t="s">
-        <v>75</v>
-      </c>
-      <c r="G81" t="s">
-        <v>215</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
       <c r="B82" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="C82" t="s">
-        <v>63</v>
-      </c>
-      <c r="E82" t="s">
-        <v>8</v>
+        <v>68</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="G82" t="s">
-        <v>124</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="B83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C83" t="s">
-        <v>68</v>
-      </c>
-      <c r="E83" t="s">
+        <v>150</v>
+      </c>
+      <c r="G83" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="B84" t="s">
+        <v>216</v>
+      </c>
+      <c r="C84" t="s">
+        <v>75</v>
+      </c>
+      <c r="G84" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="B85" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" t="s">
         <v>8</v>
       </c>
-      <c r="G83" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" t="s">
-        <v>39</v>
-      </c>
-      <c r="B85" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" t="s">
-        <v>68</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="G85" t="s">
-        <v>210</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="B86" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C86" t="s">
-        <v>113</v>
+        <v>68</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
       </c>
       <c r="G86" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="B87" t="s">
-        <v>173</v>
-      </c>
-      <c r="C87" t="s">
-        <v>113</v>
-      </c>
-      <c r="G87" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>39</v>
+      </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C88" t="s">
-        <v>100</v>
+        <v>68</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="G88" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="B89" t="s">
+        <v>172</v>
+      </c>
+      <c r="C89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G89" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="B90" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" t="s">
+        <v>113</v>
+      </c>
+      <c r="G90" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="B91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" t="s">
+        <v>100</v>
+      </c>
+      <c r="G91" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="B92" t="s">
         <v>175</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C92" t="s">
         <v>100</v>
       </c>
-      <c r="G89" s="12" t="s">
+      <c r="G92" s="12" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>